<commit_message>
New updates works on iPad!!
</commit_message>
<xml_diff>
--- a/app/Example_Files/Template; Compound Setup Table 8K Up to 32 Compunds 10 Point Dose.xlsx
+++ b/app/Example_Files/Template; Compound Setup Table 8K Up to 32 Compunds 10 Point Dose.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fulroth/Documents/Git/SPR-8K-Setup/app/Example_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D47ABF6-B550-A14F-A0BB-C274BA5AC998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{7D47ABF6-B550-A14F-A0BB-C274BA5AC998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{717489C7-485E-EC48-9CAF-939A2372147F}"/>
   <bookViews>
     <workbookView xWindow="4480" yWindow="500" windowWidth="31360" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet 1 - Table 1-1-1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -112,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1471,21 +1471,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IJ18"/>
+  <dimension ref="A1:HT18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="H1" sqref="H1:W1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.33203125" style="1" customWidth="1"/>
-    <col min="5" max="244" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.79296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.2265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.328125" style="1" customWidth="1"/>
+    <col min="5" max="228" width="10.7890625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.75" customHeight="1" thickBot="1">
+    <row r="1" spans="1:7" ht="14.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>23</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18" thickTop="1" thickBot="1">
+    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" thickTop="1" thickBot="1">
+    <row r="3" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18" thickTop="1" thickBot="1">
+    <row r="4" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18" thickTop="1" thickBot="1">
+    <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18" thickTop="1" thickBot="1">
+    <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18" thickTop="1" thickBot="1">
+    <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18" thickTop="1" thickBot="1">
+    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18" thickTop="1" thickBot="1">
+    <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>14</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16" customHeight="1" thickTop="1" thickBot="1">
+    <row r="10" spans="1:7" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>15</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" customHeight="1" thickTop="1" thickBot="1">
+    <row r="11" spans="1:7" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>16</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" customHeight="1" thickTop="1" thickBot="1">
+    <row r="12" spans="1:7" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" customHeight="1" thickTop="1" thickBot="1">
+    <row r="13" spans="1:7" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>18</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16" customHeight="1" thickTop="1" thickBot="1">
+    <row r="14" spans="1:7" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>19</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" customHeight="1" thickTop="1" thickBot="1">
+    <row r="15" spans="1:7" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>20</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" customHeight="1" thickTop="1" thickBot="1">
+    <row r="16" spans="1:7" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>21</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16" customHeight="1" thickTop="1" thickBot="1">
+    <row r="17" spans="1:7" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>22</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16" customHeight="1" thickTop="1"/>
+    <row r="18" spans="1:7" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup scale="72" orientation="portrait"/>
@@ -1772,12 +1772,12 @@
   <sheetViews>
     <sheetView zoomScale="258" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="127.6640625" customWidth="1"/>
+    <col min="1" max="1" width="127.60546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="14">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>

</xml_diff>